<commit_message>
PID tuning and config
</commit_message>
<xml_diff>
--- a/Opto 22/TSP Work.xlsx
+++ b/Opto 22/TSP Work.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ComplianceAndResearch\Opto 22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Foshizzle\ComplianceAndResearch\Opto 22\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,11 +363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313087344"/>
-        <c:axId val="313081856"/>
+        <c:axId val="245864544"/>
+        <c:axId val="245863368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313087344"/>
+        <c:axId val="245864544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,12 +424,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313081856"/>
+        <c:crossAx val="245863368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="313081856"/>
+        <c:axId val="245863368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313087344"/>
+        <c:crossAx val="245864544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,14 +1395,14 @@
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1854,13 +1854,13 @@
       <selection activeCell="F1" sqref="A1:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update required speed calculation to interpolate over the higher precision time
</commit_message>
<xml_diff>
--- a/Opto 22/TSP Work.xlsx
+++ b/Opto 22/TSP Work.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Foshizzle\ComplianceAndResearch\Opto 22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ComplianceAndResearch\Opto 22\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="10">
   <si>
     <t>Speed</t>
   </si>
@@ -199,10 +199,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -271,16 +271,46 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:f>Sheet1!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -288,66 +318,96 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,11 +423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245864544"/>
-        <c:axId val="245863368"/>
+        <c:axId val="367661208"/>
+        <c:axId val="367664344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245864544"/>
+        <c:axId val="367661208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,12 +484,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245863368"/>
+        <c:crossAx val="367664344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245863368"/>
+        <c:axId val="367664344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +546,475 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245864544"/>
+        <c:crossAx val="367661208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6580927384076991E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.89019685039370078"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="367667088"/>
+        <c:axId val="367669048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="367667088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367669048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="367669048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367667088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -575,7 +1103,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1118,6 +2202,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1389,20 +2505,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="B2" sqref="B2:B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1424,8 +2540,14 @@
       <c r="P1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1447,8 +2569,14 @@
       <c r="P2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1470,13 +2598,19 @@
       <c r="P3">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1493,13 +2627,19 @@
       <c r="P4">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1516,13 +2656,19 @@
       <c r="P5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -1539,13 +2685,19 @@
       <c r="P6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -1559,13 +2711,19 @@
       <c r="O7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <v>6</v>
@@ -1579,13 +2737,19 @@
       <c r="O8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="L9">
         <v>7</v>
@@ -1599,13 +2763,19 @@
       <c r="O9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -1619,13 +2789,19 @@
       <c r="O10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>8</v>
+      </c>
+      <c r="S10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="L11">
         <v>9</v>
@@ -1639,13 +2815,19 @@
       <c r="O11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="L12">
         <v>10</v>
@@ -1659,13 +2841,19 @@
       <c r="O12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L13">
         <v>11</v>
@@ -1679,13 +2867,19 @@
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="L14">
         <v>12</v>
@@ -1699,13 +2893,19 @@
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L15">
         <v>13</v>
@@ -1713,13 +2913,19 @@
       <c r="M15">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <v>13</v>
+      </c>
+      <c r="S15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L16">
         <v>14</v>
@@ -1727,13 +2933,19 @@
       <c r="M16">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L17">
         <v>15</v>
@@ -1741,13 +2953,19 @@
       <c r="M17">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <v>15</v>
+      </c>
+      <c r="S17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L18">
         <v>16</v>
@@ -1755,13 +2973,19 @@
       <c r="M18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <v>16</v>
+      </c>
+      <c r="S18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="L19">
         <v>17</v>
@@ -1769,13 +2993,19 @@
       <c r="M19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <v>17</v>
+      </c>
+      <c r="S19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L20">
         <v>18</v>
@@ -1783,13 +3013,19 @@
       <c r="M20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <v>18</v>
+      </c>
+      <c r="S20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L21">
         <v>19</v>
@@ -1797,13 +3033,19 @@
       <c r="M21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <v>19</v>
+      </c>
+      <c r="S21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="L22">
         <v>20</v>
@@ -1811,13 +3053,19 @@
       <c r="M22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <v>20</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L23">
         <v>21</v>
@@ -1825,18 +3073,110 @@
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <v>21</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L24">
         <v>22</v>
       </c>
       <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>22</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
         <v>0</v>
       </c>
     </row>
@@ -1854,13 +3194,13 @@
       <selection activeCell="F1" sqref="A1:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +3220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1900,7 +3240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1920,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +3280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1960,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +3320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +3340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +3380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +3400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2080,7 +3420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2100,7 +3440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2120,7 +3460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +3480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2160,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +3520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +3540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +3560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +3580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +3600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2280,7 +3620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2300,7 +3640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>

</xml_diff>